<commit_message>
Excel Finance Modeling/E.M in Corporate Finance: --> Single Cash Flow, Annuity, NPV Constant & General Discounting and Loan Amortization of Part1...[ADDED]
</commit_message>
<xml_diff>
--- a/Investing and finance lessons/Excel Finance Modeling/Excel Modeling in Corporate Finance - Craig W. Holden/Ch 02 Annuity - Ready-To-Build.xlsx
+++ b/Investing and finance lessons/Excel Finance Modeling/Excel Modeling in Corporate Finance - Craig W. Holden/Ch 02 Annuity - Ready-To-Build.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\InvestingFinance-models\Investing and finance lessons\Excel Finance Modeling\Excel Modeling in Corporate Finance - Craig W. Holden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A93FEB2-32B5-4C6E-94F3-790D5BBE9271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D12025-9CD3-4C9E-B7FB-5B73C78323FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="14400" windowHeight="15600" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="14400" windowHeight="15600" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annuity - Present Value" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>Present Value</t>
   </si>
@@ -51,18 +51,12 @@
     <t>Number of Periods</t>
   </si>
   <si>
-    <t>Present Value using a Time Line</t>
-  </si>
-  <si>
     <t>Period</t>
   </si>
   <si>
     <t>Cash Flows</t>
   </si>
   <si>
-    <t>Persent Value using the Formula</t>
-  </si>
-  <si>
     <t>Present Value using the PV Function</t>
   </si>
   <si>
@@ -136,6 +130,39 @@
   </si>
   <si>
     <t>(d) An annuity pays $40.00 each period, the appropriate discount rate / period is 6.0%, and the present value is $168.49. What is the number of periods?</t>
+  </si>
+  <si>
+    <t>Answers:</t>
+  </si>
+  <si>
+    <t>1-</t>
+  </si>
+  <si>
+    <t>2-</t>
+  </si>
+  <si>
+    <t>3-</t>
+  </si>
+  <si>
+    <t>Annuity Persent Value using the Formula</t>
+  </si>
+  <si>
+    <t>Annuity Present Value using the PV Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   a)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   d)</t>
+  </si>
+  <si>
+    <t>5 periods</t>
   </si>
 </sst>
 </file>
@@ -147,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,8 +209,23 @@
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +247,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -254,9 +302,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -268,6 +313,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,12 +619,12 @@
   <sheetData>
     <row r="2" spans="2:8" ht="30" x14ac:dyDescent="0.4">
       <c r="B2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -577,7 +633,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5">
         <v>80</v>
@@ -603,7 +659,7 @@
       <c r="B8" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <f>C19</f>
         <v>336.98910284525709</v>
       </c>
@@ -613,12 +669,12 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -641,7 +697,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
@@ -667,7 +723,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2">
@@ -716,7 +772,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -749,7 +805,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -780,7 +836,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,12 +848,12 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -806,9 +862,9 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="9">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8">
         <v>80</v>
       </c>
     </row>
@@ -830,12 +886,12 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -858,7 +914,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2">
@@ -884,7 +940,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2">
@@ -910,7 +966,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -933,7 +989,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -944,7 +1000,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" s="4">
         <f>B4*(((1+B5)^B6)-1)/B5</f>
@@ -966,7 +1022,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -977,7 +1033,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" s="4">
         <f>-FV(B5,B6,B4,0)</f>
@@ -998,7 +1054,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,10 +1065,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1022,9 +1078,9 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="14">
+        <v>9</v>
+      </c>
+      <c r="B4" s="13">
         <v>80</v>
       </c>
     </row>
@@ -1032,7 +1088,7 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>0.06</v>
       </c>
     </row>
@@ -1040,7 +1096,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <v>5</v>
       </c>
     </row>
@@ -1048,19 +1104,19 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <f>B18</f>
         <v>336.98910284525709</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -1083,7 +1139,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2">
@@ -1109,7 +1165,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2">
@@ -1145,7 +1201,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="10"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1158,7 +1214,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1191,7 +1247,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1211,12 +1267,12 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B27" s="4">
         <f>B7/((1-((1+B5)^(-B6)))/B5)</f>
@@ -1225,9 +1281,9 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="13">
+        <v>19</v>
+      </c>
+      <c r="B28" s="12">
         <f>PMT(B5,B6,-B7,0)</f>
         <v>79.999999999999986</v>
       </c>
@@ -1242,23 +1298,23 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="12">
+        <v>22</v>
+      </c>
+      <c r="B33" s="11">
         <f>RATE(B6,B28,-B7,0)</f>
         <v>6.0000000000029786E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="11">
+        <v>21</v>
+      </c>
+      <c r="B37" s="10">
         <f>NPER(B33,B28,-B24,0)</f>
         <v>5.0000000000004752</v>
       </c>
@@ -1270,55 +1326,115 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F960BE4-B237-4D5C-958D-136BC979815D}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="18" t="s">
-        <v>29</v>
+      <c r="C7" s="17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
         <v>32</v>
+      </c>
+      <c r="C15" s="4">
+        <v>734.38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4">
+        <v>319.39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4">
+        <v>179.52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="4">
+        <v>20.29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="20">
+        <v>0.32819999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>